<commit_message>
User is now able to Watch a product.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phuongthanhvan/GroupBuy_CSIT321/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196C35B4-7388-6C49-A9B6-5E9170721555}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6F2F40-E464-C642-AFE4-51EE473667AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18100" yWindow="34740" windowWidth="25440" windowHeight="15060" xr2:uid="{8D59EEA3-D85E-534C-8352-901F9ACB28FF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Tester list</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>aang_airhonker</t>
+  </si>
+  <si>
+    <t>aang_airhonker@tester.com</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,12 +501,19 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{3DDB280D-7289-2D44-8F8D-7DC1065A2058}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{9B598F73-4805-BD40-957F-0C17C8757CC5}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{A1ED0898-8C9E-6C45-99FE-22DE7A5C9292}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{17827075-951D-9645-A072-C7AA7C517122}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SingleProduct.vue - can add to watchlist
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phuongthanhvan/GroupBuy_CSIT321/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6F2F40-E464-C642-AFE4-51EE473667AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019B9496-12D7-F34E-BFF6-FFE7DFB87091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18100" yWindow="34740" windowWidth="25440" windowHeight="15060" xr2:uid="{8D59EEA3-D85E-534C-8352-901F9ACB28FF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Tester list</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>aang_airhonker@tester.com</t>
+  </si>
+  <si>
+    <t>admin@devtest.com</t>
+  </si>
+  <si>
+    <t>secret</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332FA56F-4653-634D-B93E-6226D21CBFCB}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,6 +514,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{3DDB280D-7289-2D44-8F8D-7DC1065A2058}"/>

</xml_diff>